<commit_message>
Test version of 4th update
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\飯島(データ変更厳禁)\カオイリさん 日計マクロ他資料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otabe/github.com/childhooooo/transform-daily-account/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB9901F-5AF9-4FEE-A755-3FBD454FCA88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5AB618-4034-2442-BFC4-51F2679FCAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1110" windowWidth="19065" windowHeight="14625" xr2:uid="{E6267B8B-4A21-4F96-9043-A0C6C3D02555}"/>
+    <workbookView xWindow="7320" yWindow="2240" windowWidth="14380" windowHeight="12940" xr2:uid="{E6267B8B-4A21-4F96-9043-A0C6C3D02555}"/>
   </bookViews>
   <sheets>
-    <sheet name="2回目" sheetId="2" r:id="rId1"/>
+    <sheet name="4回目" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2回目'!$A$1:$F$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'4回目'!$A$1:$F$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t>人数/件数</t>
   </si>
@@ -57,9 +58,6 @@
   </si>
   <si>
     <t>外税</t>
-  </si>
-  <si>
-    <t>内税</t>
   </si>
   <si>
     <t xml:space="preserve">消費税抜き割引前 </t>
@@ -75,9 +73,6 @@
     <t>ディナー</t>
   </si>
   <si>
-    <t>手入力</t>
-  </si>
-  <si>
     <t>消費税込</t>
   </si>
   <si>
@@ -93,9 +88,6 @@
     <t>テイク・仕出・他</t>
   </si>
   <si>
-    <t>テイク・仕出・その他外税</t>
-  </si>
-  <si>
     <t>件数</t>
   </si>
   <si>
@@ -163,12 +155,6 @@
   </si>
   <si>
     <t>売掛明細 他（当日清算済みの葬儀も含む）部門/顧客名/金額/請求日や方法を明記する</t>
-  </si>
-  <si>
-    <t>※太線枠内はデータから自動</t>
-  </si>
-  <si>
-    <t>細線枠内は手書き</t>
   </si>
   <si>
     <t>割引計</t>
@@ -200,9 +186,56 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>桐生店</t>
+    <t>人数</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>記入</t>
+    <rPh sb="0" eb="2">
+      <t>キニュウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>出前館 仕出キー</t>
     <rPh sb="0" eb="3">
-      <t>キリュウテン</t>
+      <t>デマエカン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シダシ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>内税8％テイク仕出→税抜で表示</t>
+    <rPh sb="0" eb="2">
+      <t>ウチゼイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シダ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ゼイヌキ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>税込8％仕出の内税</t>
+    <rPh sb="0" eb="2">
+      <t>ゼイコミ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シダシ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>〇〇店</t>
+    <rPh sb="2" eb="3">
+      <t xml:space="preserve">キリュウテン </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -211,10 +244,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;mm&quot;月&quot;dd&quot;日&quot;\(aaa\)"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +292,54 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +349,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -403,6 +481,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -412,7 +499,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -440,13 +527,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -476,9 +557,6 @@
     <xf numFmtId="38" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -503,9 +581,6 @@
     <xf numFmtId="38" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -515,6 +590,39 @@
     <xf numFmtId="38" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,7 +632,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -846,33 +957,34 @@
     <tabColor theme="9" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="13" style="4"/>
-    <col min="2" max="2" width="2.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="13" style="4"/>
-    <col min="5" max="5" width="16.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="13" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="21"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -888,17 +1000,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="21" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="24"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="27"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" ht="21" thickBot="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="2"/>
@@ -906,19 +1018,19 @@
       <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="28"/>
-    </row>
-    <row r="5" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" thickBot="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="28"/>
-    </row>
-    <row r="6" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" ht="21" thickBot="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="2"/>
@@ -926,492 +1038,494 @@
       <c r="E6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="28"/>
-    </row>
-    <row r="7" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" ht="21" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" ht="21" thickBot="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="6"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D8" s="8">
         <v>0.1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-      <c r="B9" s="26"/>
+        <v>8</v>
+      </c>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" ht="21" thickBot="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="8">
         <v>0.1</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" ht="23" thickBot="1">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D10" s="8">
         <v>0.1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" ht="21" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8">
         <v>0.08</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" ht="23" thickBot="1">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33" t="s">
+        <v>41</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="8">
         <v>0.1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8">
         <v>0.08</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="25"/>
+        <v>12</v>
+      </c>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" ht="23" thickBot="1">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33" t="s">
+        <v>41</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8">
         <v>0.1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8">
         <v>0.08</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="29"/>
-    </row>
-    <row r="16" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="8">
         <v>0.08</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="27"/>
-    </row>
-    <row r="17" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:6" ht="21" thickBot="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>17</v>
+      <c r="C17" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="D17" s="8">
         <v>0.08</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="30"/>
-    </row>
-    <row r="18" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1"/>
+      <c r="E17" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6" ht="21" thickBot="1">
+      <c r="A18" s="36"/>
       <c r="B18" s="1"/>
       <c r="C18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="32"/>
+        <v>15</v>
+      </c>
+      <c r="D18" s="28"/>
       <c r="E18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" ht="21" thickBot="1">
+      <c r="A19" s="36"/>
       <c r="B19" s="1"/>
       <c r="C19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="29"/>
       <c r="E19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="28"/>
-    </row>
-    <row r="20" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:6" ht="21" thickBot="1">
+      <c r="A20" s="37"/>
       <c r="B20" s="1"/>
       <c r="C20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="28"/>
-    </row>
-    <row r="21" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="1"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="1:6" ht="21" thickBot="1">
+      <c r="A21" s="36"/>
       <c r="B21" s="1"/>
       <c r="C21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D21" s="29"/>
       <c r="E21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="F21" s="25"/>
+    </row>
+    <row r="22" spans="1:6" ht="21" thickBot="1">
+      <c r="A22" s="38"/>
       <c r="B22" s="1"/>
       <c r="C22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D22" s="29"/>
       <c r="E22" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="F22" s="25"/>
+    </row>
+    <row r="23" spans="1:6" ht="21" thickBot="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D23" s="29"/>
       <c r="E23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="24" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="1:6" ht="21" thickBot="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D24" s="29"/>
       <c r="E24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="28"/>
-    </row>
-    <row r="25" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="1:6" ht="21" thickBot="1">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="25"/>
+    </row>
+    <row r="26" spans="1:6" ht="21" thickBot="1">
+      <c r="A26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="13" t="s">
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="1:6" ht="21" thickBot="1">
+      <c r="A27" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15" t="s">
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:6" ht="21" thickBot="1">
+      <c r="A28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" spans="1:6" ht="21" thickBot="1">
+      <c r="A29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="F29" s="25"/>
+    </row>
+    <row r="30" spans="1:6" ht="21" thickBot="1">
+      <c r="A30" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="28"/>
-    </row>
-    <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="F30" s="25"/>
+    </row>
+    <row r="31" spans="1:6" ht="21" thickBot="1">
+      <c r="A31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="F31" s="25"/>
+    </row>
+    <row r="32" spans="1:6" ht="21" thickBot="1">
+      <c r="A32" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="28"/>
-    </row>
-    <row r="30" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="7" t="s">
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" ht="21" thickBot="1">
+      <c r="A33" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="28"/>
-    </row>
-    <row r="31" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="7" t="s">
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:6" ht="21" thickBot="1">
+      <c r="A34" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="28"/>
-    </row>
-    <row r="32" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="7" t="s">
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="28"/>
-    </row>
-    <row r="33" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="7" t="s">
+      <c r="F35" s="26"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="28"/>
-    </row>
-    <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="28"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A35" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="29"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A36" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="31"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A38" s="34"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A39" s="1"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="1:6" ht="21.75" customHeight="1">
+      <c r="A37" s="41"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:6" ht="21.75" customHeight="1">
+      <c r="A38" s="41"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="39"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="20"/>
+      <c r="E39" s="18"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
-      </c>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="23"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="20"/>
+      <c r="E40" s="18"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="20"/>
+      <c r="E41" s="18"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="2"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="20"/>
+      <c r="E42" s="18"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="20"/>
+      <c r="E43" s="18"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="18"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:6">
+      <c r="A45" s="39"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="20"/>
+      <c r="E45" s="18"/>
       <c r="F45" s="2"/>
     </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="40"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A37:F37"/>
     <mergeCell ref="A38:F38"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>

<commit_message>
Upgrade packages and change calclulation methods
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otabe/github.com/kaoiri/transform-daily-account/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hikaru/github.com/kaoiri/transform-daily-account/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9496FED-5BCC-074A-9CF6-2AE646548DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A07BC39-2FE2-DF4C-9C29-1B5C1F176F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="5380" xr2:uid="{E6267B8B-4A21-4F96-9043-A0C6C3D02555}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="26840" windowHeight="17600" xr2:uid="{E6267B8B-4A21-4F96-9043-A0C6C3D02555}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
   <si>
     <t>人数/件数</t>
   </si>
@@ -124,13 +124,6 @@
   </si>
   <si>
     <t>外税</t>
-  </si>
-  <si>
-    <t xml:space="preserve">消費税抜き割引前 </t>
-    <rPh sb="7" eb="8">
-      <t>マエ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>ランチ</t>
@@ -273,22 +266,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>内税8％テイク仕出→税抜で表示</t>
-    <rPh sb="0" eb="2">
-      <t>ウチゼイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>シダ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ゼイヌキ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>税込8％仕出の内税</t>
     <rPh sb="0" eb="2">
       <t>ゼイコミ</t>
@@ -358,6 +335,40 @@
   </si>
   <si>
     <t>人時売上</t>
+  </si>
+  <si>
+    <t xml:space="preserve">消費税込割引前 </t>
+    <rPh sb="6" eb="7">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">消費税込割引前 </t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">コミ </t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>消費税込</t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">コミ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>内税8％テイク仕出</t>
+    <rPh sb="0" eb="2">
+      <t>ウチゼイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シダ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -784,7 +795,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -848,22 +859,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -878,7 +880,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -911,34 +913,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="13" fillId="2" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="13" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="13" fillId="5" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="6" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="6" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -947,10 +949,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="8" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,10 +961,10 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="10" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="10" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -971,10 +973,10 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="12" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="12" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="12" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -983,31 +985,31 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="14" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="14" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="13" fillId="15" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="15" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="13" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="16" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="5" fillId="16" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="13" fillId="17" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="16" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="13" fillId="17" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="5" fillId="17" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="13" fillId="18" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="13" fillId="18" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1347,8 +1349,8 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="136" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="20"/>
@@ -1366,69 +1368,69 @@
     <row r="1" spans="1:26" ht="21" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="75"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="39" t="s">
+      <c r="L1" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="M1" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="N1" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="O1" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="P1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="Q1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="R1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="S1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="T1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="U1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="V1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="W1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="X1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="Y1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="Z1" s="36" t="s">
         <v>60</v>
-      </c>
-      <c r="Y1" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z1" s="39" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="21" thickBot="1">
@@ -1446,44 +1448,86 @@
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="56">
+      <c r="H2" s="40">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="41">
+        <f>F4</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="43">
+        <f>F8</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="45">
+        <f>A8</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="47">
+        <f>F9</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="49">
+        <f>A9</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="51">
+        <f>(F10+F11)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="53">
         <f>A10</f>
         <v>0</v>
       </c>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="60">
+      <c r="P2" s="55">
+        <f>(F12+F13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="57">
         <f>A12</f>
         <v>0</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="64">
+      <c r="R2" s="59">
+        <f>(F14+F15)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="61">
         <f>A14</f>
         <v>0</v>
       </c>
-      <c r="T2" s="66"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="41"/>
+      <c r="T2" s="63">
+        <f>F16</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="65">
+        <f>F17</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="71">
+        <f>(F16 + F17)</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="67">
+        <f>F22</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="69">
+        <f>D22</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="38"/>
     </row>
     <row r="3" spans="1:26" ht="21" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="21"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="42"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:26" ht="21" thickBot="1">
       <c r="A4" s="5"/>
@@ -1493,7 +1537,7 @@
       <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="21" thickBot="1">
       <c r="A5" s="5"/>
@@ -1501,9 +1545,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="25"/>
+        <v>38</v>
+      </c>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:26" ht="21" thickBot="1">
       <c r="A6" s="5"/>
@@ -1513,432 +1557,432 @@
       <c r="E6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:26" ht="21" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="25"/>
+      <c r="E7" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:26" ht="21" thickBot="1">
-      <c r="A8" s="49"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="D8" s="8">
         <v>0.1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="47"/>
+        <v>7</v>
+      </c>
+      <c r="F8" s="44"/>
     </row>
     <row r="9" spans="1:26" ht="21" thickBot="1">
-      <c r="A9" s="53"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D9" s="8">
         <v>0.1</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="48"/>
+    </row>
+    <row r="10" spans="1:26" ht="23" thickBot="1">
+      <c r="A10" s="54"/>
+      <c r="B10" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F9" s="51"/>
-    </row>
-    <row r="10" spans="1:26" ht="23" thickBot="1">
-      <c r="A10" s="57"/>
-      <c r="B10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D10" s="8">
         <v>0.1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" ht="21" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="8">
         <v>0.08</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="25"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:26" ht="23" thickBot="1">
-      <c r="A12" s="61"/>
-      <c r="B12" s="31" t="s">
-        <v>41</v>
+      <c r="A12" s="58"/>
+      <c r="B12" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="8">
         <v>0.1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="59"/>
+        <v>11</v>
+      </c>
+      <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="21" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="8">
         <v>0.08</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="25"/>
+        <v>11</v>
+      </c>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:26" ht="23" thickBot="1">
-      <c r="A14" s="65"/>
-      <c r="B14" s="31" t="s">
-        <v>41</v>
+      <c r="A14" s="62"/>
+      <c r="B14" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="8">
         <v>0.1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:26" ht="21" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="8">
         <v>0.08</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="26"/>
+        <v>12</v>
+      </c>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:26" ht="21" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D16" s="8">
         <v>0.08</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="67"/>
+        <v>13</v>
+      </c>
+      <c r="F16" s="64"/>
     </row>
     <row r="17" spans="1:6" ht="21" thickBot="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="32" t="s">
-        <v>43</v>
+      <c r="C17" s="31" t="s">
+        <v>64</v>
       </c>
       <c r="D17" s="8">
         <v>0.08</v>
       </c>
-      <c r="E17" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="69"/>
+      <c r="E17" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="66"/>
     </row>
     <row r="18" spans="1:6" ht="21" thickBot="1">
-      <c r="A18" s="34"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="1"/>
       <c r="C18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="1:6" ht="21" thickBot="1">
-      <c r="A19" s="34"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1"/>
       <c r="C19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="26"/>
       <c r="E19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="25"/>
+        <v>16</v>
+      </c>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" ht="21" thickBot="1">
-      <c r="A20" s="35"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="1"/>
       <c r="C20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="D20" s="26"/>
       <c r="E20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" ht="21" thickBot="1">
-      <c r="A21" s="34"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="1"/>
       <c r="C21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="D21" s="26"/>
       <c r="E21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="25"/>
+        <v>18</v>
+      </c>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="21" thickBot="1">
-      <c r="A22" s="36"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="1"/>
       <c r="C22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="73"/>
+        <v>14</v>
+      </c>
+      <c r="D22" s="70"/>
       <c r="E22" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="71"/>
+        <v>37</v>
+      </c>
+      <c r="F22" s="68"/>
     </row>
     <row r="23" spans="1:6" ht="21" thickBot="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="D23" s="26"/>
       <c r="E23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="25"/>
+        <v>19</v>
+      </c>
+      <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="21" thickBot="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="D24" s="26"/>
       <c r="E24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="25"/>
+        <v>20</v>
+      </c>
+      <c r="F24" s="22"/>
     </row>
     <row r="25" spans="1:6" ht="21" thickBot="1">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="25"/>
+      <c r="F25" s="22"/>
     </row>
     <row r="26" spans="1:6" ht="21" thickBot="1">
       <c r="A26" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="25"/>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:6" ht="21" thickBot="1">
       <c r="A27" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="15"/>
       <c r="D27" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="25"/>
+        <v>27</v>
+      </c>
+      <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:6" ht="21" thickBot="1">
       <c r="A28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="15"/>
       <c r="D28" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" ht="21" thickBot="1">
       <c r="A29" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="15"/>
       <c r="D29" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="25"/>
+        <v>29</v>
+      </c>
+      <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:6" ht="21" thickBot="1">
       <c r="A30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="15"/>
       <c r="D30" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="25"/>
+        <v>30</v>
+      </c>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:6" ht="21" thickBot="1">
       <c r="A31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="15"/>
       <c r="D31" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="25"/>
+        <v>31</v>
+      </c>
+      <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:6" ht="21" thickBot="1">
       <c r="A32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B32" s="2"/>
       <c r="C32" s="15"/>
       <c r="D32" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="25"/>
+        <v>32</v>
+      </c>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" ht="21" thickBot="1">
       <c r="A33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B33" s="2"/>
       <c r="C33" s="15"/>
       <c r="D33" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="25"/>
+        <v>33</v>
+      </c>
+      <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" ht="21" thickBot="1">
       <c r="A34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B34" s="2"/>
       <c r="C34" s="15"/>
       <c r="D34" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="25"/>
+        <v>34</v>
+      </c>
+      <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B35" s="2"/>
       <c r="C35" s="16"/>
       <c r="D35" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" s="26"/>
+        <v>35</v>
+      </c>
+      <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="22"/>
+        <v>36</v>
+      </c>
+      <c r="B36" s="1"/>
       <c r="C36" s="19"/>
       <c r="D36" s="15"/>
       <c r="E36" s="17"/>
-      <c r="F36" s="27"/>
+      <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:6" ht="21.75" customHeight="1">
-      <c r="A37" s="75"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="77"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="74"/>
     </row>
     <row r="38" spans="1:6" ht="21.75" customHeight="1">
-      <c r="A38" s="75"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="77"/>
+      <c r="A38" s="72"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="74"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="37"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2"/>
       <c r="D39" s="1"/>
@@ -1986,7 +2030,7 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="37"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
       <c r="D45" s="1"/>
@@ -1994,7 +2038,7 @@
       <c r="F45" s="2"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="38"/>
+      <c r="A48" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>